<commit_message>
Objectives to turn light on working again
</commit_message>
<xml_diff>
--- a/Assets/Script/Puzzling/quests.xlsx
+++ b/Assets/Script/Puzzling/quests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Unity\GDTVJam\Assets\Script\Puzzling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D35336A-1DCE-41E6-AAD3-5D73D5243E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991D3547-9717-4EB3-9394-C2EB4866A480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B998B016-64FD-483C-AD6C-3A8C9C9EBEEB}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="118">
   <si>
     <t>ID</t>
   </si>
@@ -172,9 +172,6 @@
     <t>Find chemical to make a lock melter</t>
   </si>
   <si>
-    <t>Send found chemical to Player1</t>
-  </si>
-  <si>
     <t>Find a pen&amp;paper</t>
   </si>
   <si>
@@ -205,12 +202,6 @@
     <t>Inspect a car</t>
   </si>
   <si>
-    <t>Give a list of items to Player1</t>
-  </si>
-  <si>
-    <t>Take a wishlist of items from Player2</t>
-  </si>
-  <si>
     <t>Find an equipment to fix a car</t>
   </si>
   <si>
@@ -359,6 +350,39 @@
   </si>
   <si>
     <t>}</t>
+  </si>
+  <si>
+    <t>Give a list of wanted equipment to Player1</t>
+  </si>
+  <si>
+    <t>Take a wishlist from Player2</t>
+  </si>
+  <si>
+    <t>Take a key on a car</t>
+  </si>
+  <si>
+    <t>Unlock bedroom 2</t>
+  </si>
+  <si>
+    <t>P1UnlockBedroom1</t>
+  </si>
+  <si>
+    <t>P1UnlockBedroom2</t>
+  </si>
+  <si>
+    <t>Send found chemical to Player2</t>
+  </si>
+  <si>
+    <t>P2SendChemicalsToP2</t>
+  </si>
+  <si>
+    <t>P2MixLockMelter</t>
+  </si>
+  <si>
+    <t>P1TakeLockMelter</t>
+  </si>
+  <si>
+    <t>Get a lock melter from Player2</t>
   </si>
 </sst>
 </file>
@@ -476,7 +500,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="13">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -494,6 +518,80 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -893,10 +991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82CBC90A-0F48-49AA-AFB1-7CD57B4EF7AE}">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -904,7 +1002,7 @@
     <col min="1" max="1" width="7" style="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" customWidth="1"/>
     <col min="3" max="3" width="36.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" customWidth="1"/>
     <col min="6" max="6" width="23" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -920,7 +1018,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -947,7 +1045,7 @@
         <v>301</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>7</v>
@@ -974,7 +1072,7 @@
         <v>399</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>8</v>
@@ -1001,7 +1099,7 @@
         <v>375</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>9</v>
@@ -1028,7 +1126,7 @@
         <v>305</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>10</v>
@@ -1055,7 +1153,7 @@
         <v>209</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>7</v>
@@ -1082,7 +1180,7 @@
         <v>117</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>11</v>
@@ -1109,7 +1207,7 @@
         <v>136</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>41</v>
@@ -1136,7 +1234,7 @@
         <v>305</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>42</v>
@@ -1163,7 +1261,7 @@
         <v>411</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>43</v>
@@ -1190,10 +1288,10 @@
         <v>361</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>39</v>
@@ -1217,10 +1315,10 @@
         <v>176</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>40</v>
@@ -1244,7 +1342,7 @@
         <v>144</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>44</v>
@@ -1271,7 +1369,7 @@
         <v>347</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>45</v>
@@ -1298,10 +1396,10 @@
         <v>51</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>40</v>
@@ -1325,10 +1423,10 @@
         <v>474</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>39</v>
@@ -1352,10 +1450,10 @@
         <v>420:249:485:185:115:153</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>39</v>
@@ -1378,7 +1476,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>46</v>
@@ -1404,7 +1502,7 @@
         <v>0</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>46</v>
@@ -1430,7 +1528,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>46</v>
@@ -1457,7 +1555,7 @@
         <v>153</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>46</v>
@@ -1484,7 +1582,7 @@
         <v>153</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>46</v>
@@ -1507,11 +1605,11 @@
         <v>115</v>
       </c>
       <c r="B23" s="4">
-        <f t="shared" ref="B23:B31" si="1">A24</f>
+        <f t="shared" ref="B23:B30" si="1">A24</f>
         <v>153</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>46</v>
@@ -1538,16 +1636,16 @@
         <v>325</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>47</v>
+        <v>113</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G24" s="4">
         <v>0</v>
@@ -1561,20 +1659,20 @@
         <v>325</v>
       </c>
       <c r="B25" s="4">
-        <f t="shared" si="1"/>
-        <v>64</v>
+        <f>A26</f>
+        <v>28</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="G25" s="4">
         <v>0</v>
@@ -1585,131 +1683,131 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
+        <v>28</v>
+      </c>
+      <c r="B26" s="4">
+        <f>A27</f>
         <v>64</v>
       </c>
-      <c r="B26" s="4">
+      <c r="C26" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="4">
+        <v>0</v>
+      </c>
+      <c r="H26" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="4">
+        <v>64</v>
+      </c>
+      <c r="B27" s="4">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C27" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="4">
+        <v>0</v>
+      </c>
+      <c r="H27" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="4">
         <v>90</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" s="4">
-        <v>0</v>
-      </c>
-      <c r="H26" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="4">
-        <v>90</v>
-      </c>
-      <c r="B27" s="4">
+      <c r="B28" s="4">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E27" s="4" t="s">
+      <c r="C28" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F28" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G27" s="4">
-        <v>0</v>
-      </c>
-      <c r="H27" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="4">
+      <c r="G28" s="4">
+        <v>0</v>
+      </c>
+      <c r="H28" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="4">
         <v>110</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B29" s="4">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28" s="4" t="s">
+      <c r="C29" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F29" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G28" s="4">
-        <v>0</v>
-      </c>
-      <c r="H28" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="4">
+      <c r="G29" s="4">
+        <v>0</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="4">
         <v>2</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B30" s="4">
         <f t="shared" si="1"/>
         <v>273</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G29" s="4">
-        <v>0</v>
-      </c>
-      <c r="H29" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="4">
-        <v>273</v>
-      </c>
-      <c r="B30" s="4">
-        <f t="shared" si="1"/>
-        <v>455</v>
-      </c>
       <c r="C30" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>40</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="G30" s="4">
         <v>0</v>
@@ -1720,17 +1818,17 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
+        <v>273</v>
+      </c>
+      <c r="B31" s="4">
+        <f>A32</f>
         <v>455</v>
       </c>
-      <c r="B31" s="4">
-        <f t="shared" si="1"/>
-        <v>75</v>
-      </c>
       <c r="C31" s="9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>40</v>
@@ -1747,20 +1845,20 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
+        <v>455</v>
+      </c>
+      <c r="B32" s="4">
+        <f>A33</f>
         <v>75</v>
       </c>
-      <c r="B32" s="7" t="str">
-        <f>_xlfn.TEXTJOIN(":",TRUE, A33:A36)</f>
-        <v>95:326:439:412</v>
-      </c>
       <c r="C32" s="9" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>22</v>
@@ -1774,23 +1872,23 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
-        <v>95</v>
-      </c>
-      <c r="B33" s="4">
-        <f>A37</f>
-        <v>389</v>
+        <v>75</v>
+      </c>
+      <c r="B33" s="7" t="str">
+        <f>_xlfn.TEXTJOIN(":",TRUE, A36:A38,A34)</f>
+        <v>95:326:439:67</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G33" s="4">
         <v>0</v>
@@ -1801,23 +1899,23 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
-        <v>326</v>
-      </c>
-      <c r="B34" s="4">
-        <f>A37</f>
-        <v>389</v>
+        <v>67</v>
+      </c>
+      <c r="B34" s="7">
+        <f>A35</f>
+        <v>68</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>62</v>
+        <v>109</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="G34" s="4">
         <v>0</v>
@@ -1828,23 +1926,23 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
-        <v>439</v>
-      </c>
-      <c r="B35" s="4">
-        <f>A37</f>
-        <v>389</v>
+        <v>68</v>
+      </c>
+      <c r="B35" s="7">
+        <f>A39</f>
+        <v>412</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="G35" s="4">
         <v>0</v>
@@ -1855,23 +1953,23 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
-        <v>412</v>
+        <v>95</v>
       </c>
       <c r="B36" s="4">
-        <f>A37</f>
+        <f>A40</f>
         <v>389</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>101</v>
+        <v>58</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="G36" s="4">
         <v>0</v>
@@ -1882,23 +1980,23 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="4">
+        <v>326</v>
+      </c>
+      <c r="B37" s="4">
+        <f>A40</f>
         <v>389</v>
       </c>
-      <c r="B37" s="7" t="str">
-        <f>_xlfn.TEXTJOIN(":",TRUE,A38:A39)</f>
-        <v>228:303</v>
-      </c>
       <c r="C37" s="9" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="G37" s="4">
         <v>0</v>
@@ -1909,19 +2007,20 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
-        <v>228</v>
+        <v>439</v>
       </c>
       <c r="B38" s="4">
-        <v>0</v>
+        <f>A40</f>
+        <v>389</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>22</v>
@@ -1935,42 +2034,135 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
+        <v>412</v>
+      </c>
+      <c r="B39" s="4">
+        <f>A40</f>
+        <v>389</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G39" s="4">
+        <v>0</v>
+      </c>
+      <c r="H39" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" s="4">
+        <v>389</v>
+      </c>
+      <c r="B40" s="7" t="str">
+        <f>_xlfn.TEXTJOIN(":",TRUE,A41:A42)</f>
+        <v>228:303</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G40" s="4">
+        <v>0</v>
+      </c>
+      <c r="H40" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" s="4">
+        <v>228</v>
+      </c>
+      <c r="B41" s="4">
+        <v>0</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41" s="4">
+        <v>0</v>
+      </c>
+      <c r="H41" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" s="4">
         <v>303</v>
       </c>
-      <c r="B39" s="4">
-        <v>0</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E39" s="4" t="s">
+      <c r="B42" s="4">
+        <v>0</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="F42" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G39" s="4">
-        <v>0</v>
-      </c>
-      <c r="H39" s="4">
+      <c r="G42" s="4">
+        <v>0</v>
+      </c>
+      <c r="H42" s="4">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="endsWith" dxfId="4" priority="4" operator="endsWith" text="1">
+  <conditionalFormatting sqref="E1:E34 E36:E1048576">
+    <cfRule type="endsWith" dxfId="9" priority="9" operator="endsWith" text="1">
       <formula>RIGHT(E1,LEN("1"))="1"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+  <conditionalFormatting sqref="A36:A1048576 A1:A34">
+    <cfRule type="duplicateValues" dxfId="8" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C39">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  <conditionalFormatting sqref="C2:C34 C36:C42">
+    <cfRule type="duplicateValues" dxfId="6" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule type="endsWith" dxfId="5" priority="3" operator="endsWith" text="1">
+      <formula>RIGHT(E35,LEN("1"))="1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35">
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2010,7 +2202,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2211,539 +2403,539 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C2" s="13">
         <v>203</v>
       </c>
       <c r="D2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C3" s="13">
         <v>301</v>
       </c>
       <c r="D3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C4" s="13">
         <v>399</v>
       </c>
       <c r="D4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C5" s="13">
         <v>375</v>
       </c>
       <c r="D5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C6" s="13">
         <v>208</v>
       </c>
       <c r="D6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C7" s="13">
         <v>209</v>
       </c>
       <c r="D7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C8" s="13">
         <v>117</v>
       </c>
       <c r="D8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C9" s="13">
         <v>136</v>
       </c>
       <c r="D9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C10" s="13">
         <v>305</v>
       </c>
       <c r="D10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C11" s="13">
         <v>411</v>
       </c>
       <c r="D11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C12" s="13">
         <v>361</v>
       </c>
       <c r="D12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C13" s="13">
         <v>176</v>
       </c>
       <c r="D13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C14" s="13">
         <v>144</v>
       </c>
       <c r="D14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C15" s="13">
         <v>347</v>
       </c>
       <c r="D15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C16" s="13">
         <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C17" s="13">
         <v>474</v>
       </c>
       <c r="D17" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C18" s="13">
         <v>179</v>
       </c>
       <c r="D18" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C19" s="13">
         <v>420</v>
       </c>
       <c r="D19" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C20" s="13">
         <v>249</v>
       </c>
       <c r="D20" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C21" s="13">
         <v>485</v>
       </c>
       <c r="D21" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C22" s="13">
         <v>185</v>
       </c>
       <c r="D22" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C23" s="13">
         <v>115</v>
       </c>
       <c r="D23" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C24" s="13">
         <v>153</v>
       </c>
       <c r="D24" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C25" s="13">
         <v>325</v>
       </c>
       <c r="D25" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C26" s="13">
         <v>64</v>
       </c>
       <c r="D26" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C27" s="13">
         <v>90</v>
       </c>
       <c r="D27" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C28" s="13">
         <v>110</v>
       </c>
       <c r="D28" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C29" s="13">
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C30" s="13">
         <v>273</v>
       </c>
       <c r="D30" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A31" s="11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C31" s="13">
         <v>455</v>
       </c>
       <c r="D31" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C32" s="13">
         <v>75</v>
       </c>
       <c r="D32" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C33" s="13">
         <v>95</v>
       </c>
       <c r="D33" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C34" s="13">
         <v>326</v>
       </c>
       <c r="D34" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C35" s="13">
         <v>439</v>
       </c>
       <c r="D35" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C36" s="13">
         <v>412</v>
       </c>
       <c r="D36" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C37" s="13">
         <v>389</v>
       </c>
       <c r="D37" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A38" s="11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C38" s="13">
         <v>228</v>
       </c>
       <c r="D38" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A39" s="11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C39" s="13">
         <v>303</v>
       </c>
       <c r="D39" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Open art room objective
Script arrangement
</commit_message>
<xml_diff>
--- a/Assets/Script/Puzzling/quests.xlsx
+++ b/Assets/Script/Puzzling/quests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Unity\GDTVJam\Assets\Script\Puzzling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991D3547-9717-4EB3-9394-C2EB4866A480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE11D20-28F6-43FF-AA38-D30B8D3D155B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B998B016-64FD-483C-AD6C-3A8C9C9EBEEB}"/>
   </bookViews>
@@ -500,7 +500,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -565,33 +565,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -993,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82CBC90A-0F48-49AA-AFB1-7CD57B4EF7AE}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1256,9 +1229,9 @@
       <c r="A10" s="4">
         <v>305</v>
       </c>
-      <c r="B10" s="4">
-        <f t="shared" si="0"/>
-        <v>411</v>
+      <c r="B10" s="4" t="str">
+        <f>_xlfn.TEXTJOIN(":",TRUE, A11:A12)</f>
+        <v>411:361</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>71</v>
@@ -1284,8 +1257,7 @@
         <v>411</v>
       </c>
       <c r="B11" s="4">
-        <f t="shared" si="0"/>
-        <v>361</v>
+        <v>0</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>72</v>
@@ -1311,8 +1283,7 @@
         <v>361</v>
       </c>
       <c r="B12" s="4">
-        <f t="shared" si="0"/>
-        <v>176</v>
+        <v>144</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>73</v>

</xml_diff>